<commit_message>
modified homoGraphBuilder.cpp and result.xlsx
</commit_message>
<xml_diff>
--- a/experiment/Result Analysis.xlsx
+++ b/experiment/Result Analysis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\84097\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA29274E-E1B3-4E29-8E8F-FBF75467D7E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96246967-F2AE-4C9F-A75A-0808D44F6777}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="24196" windowHeight="14476" xr2:uid="{C787EE50-9488-4076-9B3E-6C4BBE8FA416}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="97">
   <si>
     <t>DBLP</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -254,74 +254,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>num of P = 513278
-"1 1 0 2 2 3 0 0 1"=82020233us</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>num of T = 84323
-"1 1 0 2 2 3 0 0 1"=738662us</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>num of [1] = 1186
-"3 5 0 0 1 3 0 2 3"=359815us</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>num of [2] = 5348
-"3 5 0 0 1 3 0 2 3"=110894us</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>num of [1] = 4803
-"1 1 0 2 2 3 0 0 1"=1815658us</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>num of [2] = 88
-"1 1 0 2 2 3 0 0 1"=49808us</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>num of [1] = 409340
-"1 3 0 2 3 5 0 0 1"=155026118us</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>num of [2] = 66019
-"1 3 0 2 3 5 0 0 1"=493554us</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>6425064us</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>189731us</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>454035965us</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>713689us</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>512213us</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>10267408us</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>46812595us</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>[1] join analysis</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -353,10 +285,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>11064594us</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>total: 91,350,165
 useful: 82,611,016
 useless: 8,739,149</t>
@@ -384,6 +312,162 @@
     <t>total: 14,728,291
 useful: 474,144
 useless: 14,254,147</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>num of P = 513278
+"1 1 0 2 2 3 0 0 1"=82,020,233us</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>6,425,064us</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>num of T = 84323
+"1 1 0 2 2 3 0 0 1"=738,662us</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>713,689us</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>num of [1] = 1186
+"3 5 0 0 1 3 0 2 3"=359,815us</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>189,731us</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>num of [2] = 5348
+"3 5 0 0 1 3 0 2 3"=110,894us</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>512,213us</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>num of [1] = 4803
+"1 1 0 2 2 3 0 0 1"=1,815,658us</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>11,064,594us</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>num of [2] = 88
+"1 1 0 2 2 3 0 0 1"=49,808us</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>10,267,408us</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>num of [1] = 409340
+"1 3 0 2 3 5 0 0 1"=155,026,118us</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>454,035,965us</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>num of [2] = 66019
+"1 3 0 2 3 5 0 0 1"=493,554us</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>46,812,595us</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>以[1]为分点，估算join次数所需要的时间</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>”1 1 0 2 2 3 0 0 1“=1,327,271us</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>以[2]为分点，估算join次数所需要的时间</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>”1 1 0 2 2 3 0 0 1“=1,178,846us</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>”1 1 0 2 2 3 0 0 1“=58,319us</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>”1 1 0 2 2 3 0 0 1“=44,329us</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>"3 5 0 0 1 3 0 2 3"=7,536us</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>"3 5 0 0 1 3 0 2 3"=8,504us</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>"1 3 0 2 3 5 0 0 1"=1,335,388us</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>"1 3 0 2 3 5 0 0 1"=1,249,994us</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[0] 查找所需要的时间</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[0] Join所需要的时间</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>num of A = 54881
+"1 1 0 2 2 3  0 0 1"=5,515,450us</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>num of [0] = 54588
+"1 1 0 2 2 3 0 0 1"=19,295,988us</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>22,835,536us</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>231,500us</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>106,670us</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>num of [0] = 886
+"3 5 0 0 1 3 0 2 3"=375,142us</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>num of [0] = 402154
+"1 3 0 2 3 5 0 0 1"=158,848,148us</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>86,659,332us</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1044,10 +1128,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:T9"/>
+  <dimension ref="A1:X9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O2" zoomScale="102" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="U3" sqref="U3"/>
+    <sheetView tabSelected="1" zoomScale="86" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
@@ -1062,17 +1146,17 @@
     <col min="8" max="10" width="30.796875" customWidth="1"/>
     <col min="11" max="12" width="31.59765625" style="2" customWidth="1"/>
     <col min="13" max="13" width="27.59765625" style="2" customWidth="1"/>
-    <col min="14" max="14" width="31.59765625" style="2" customWidth="1"/>
-    <col min="15" max="15" width="29.73046875" customWidth="1"/>
-    <col min="16" max="16" width="28.86328125" style="3" customWidth="1"/>
-    <col min="17" max="17" width="28.86328125" customWidth="1"/>
-    <col min="18" max="18" width="28.86328125" style="4" customWidth="1"/>
-    <col min="19" max="19" width="26.46484375" customWidth="1"/>
-    <col min="20" max="20" width="24.86328125" customWidth="1"/>
-    <col min="21" max="21" width="15.6640625" customWidth="1"/>
+    <col min="14" max="16" width="31.59765625" style="2" customWidth="1"/>
+    <col min="17" max="17" width="29.73046875" customWidth="1"/>
+    <col min="18" max="18" width="28.86328125" style="3" customWidth="1"/>
+    <col min="19" max="19" width="28.86328125" customWidth="1"/>
+    <col min="20" max="20" width="28.86328125" style="4" customWidth="1"/>
+    <col min="21" max="21" width="26.46484375" customWidth="1"/>
+    <col min="22" max="22" width="24.86328125" customWidth="1"/>
+    <col min="23" max="24" width="35.53125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:24" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
         <v>4</v>
       </c>
@@ -1116,25 +1200,37 @@
         <v>30</v>
       </c>
       <c r="O1" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="Q1" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="P1" s="3" t="s">
+      <c r="R1" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="S1" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="R1" s="4" t="s">
+      <c r="T1" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="S1" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="T1" s="2" t="s">
-        <v>66</v>
+      <c r="U1" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="V1" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="W1" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="X1" s="2" t="s">
+        <v>79</v>
       </c>
     </row>
-    <row r="2" spans="1:20" ht="135.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:24" ht="135.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -1175,25 +1271,37 @@
         <v>16</v>
       </c>
       <c r="O2" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="P2" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="P2" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="Q2" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="R2" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="S2" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="T2" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="U2" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="V2" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="Q2" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="R2" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="S2" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="T2" s="5" t="s">
-        <v>74</v>
+      <c r="W2" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="X2" s="5" t="s">
+        <v>80</v>
       </c>
     </row>
-    <row r="3" spans="1:20" ht="135.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:24" ht="135.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -1234,25 +1342,37 @@
         <v>17</v>
       </c>
       <c r="O3" s="3" t="s">
-        <v>52</v>
+        <v>94</v>
       </c>
       <c r="P3" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="Q3" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="R3" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="S3" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="T3" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="U3" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="Q3" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="R3" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="S3" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="T3" s="5" t="s">
-        <v>76</v>
+      <c r="V3" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="W3" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="X3" s="5" t="s">
+        <v>84</v>
       </c>
     </row>
-    <row r="4" spans="1:20" ht="135.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:24" ht="135.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A4" s="2" t="s">
         <v>11</v>
       </c>
@@ -1275,7 +1395,7 @@
         <v>40</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>70</v>
+        <v>55</v>
       </c>
       <c r="J4" s="3" t="s">
         <v>41</v>
@@ -1293,25 +1413,37 @@
         <v>23</v>
       </c>
       <c r="O4" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="P4" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="Q4" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="R4" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="S4" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="T4" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="U4" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="P4" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="Q4" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="R4" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="S4" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="T4" s="5" t="s">
-        <v>72</v>
+      <c r="V4" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="W4" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="X4" s="5" t="s">
+        <v>82</v>
       </c>
     </row>
-    <row r="5" spans="1:20" ht="135.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:24" ht="135.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A5" s="2" t="s">
         <v>0</v>
       </c>
@@ -1352,25 +1484,37 @@
         <v>21</v>
       </c>
       <c r="O5" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="P5" s="4" t="s">
-        <v>60</v>
+        <v>95</v>
+      </c>
+      <c r="P5" s="3" t="s">
+        <v>96</v>
       </c>
       <c r="Q5" s="3" t="s">
-        <v>57</v>
+        <v>73</v>
       </c>
       <c r="R5" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="S5" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="T5" s="5" t="s">
-        <v>67</v>
+        <v>74</v>
+      </c>
+      <c r="S5" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="T5" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="U5" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="V5" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="W5" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="X5" s="5" t="s">
+        <v>86</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.4">
       <c r="A6" s="2" t="s">
         <v>2</v>
       </c>
@@ -1390,7 +1534,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.4">
       <c r="A7" s="2" t="s">
         <v>12</v>
       </c>
@@ -1410,7 +1554,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="8" spans="1:20" ht="135" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:24" ht="135" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A8" s="2" t="s">
         <v>0</v>
       </c>
@@ -1433,7 +1577,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:20" ht="135.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:24" ht="135.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A9" s="2" t="s">
         <v>1</v>
       </c>

</xml_diff>